<commit_message>
report add max/avg men,cpu
</commit_message>
<xml_diff>
--- a/testRunner/report.xlsx
+++ b/testRunner/report.xlsx
@@ -47,7 +47,7 @@
     <t>'2.2.8'</t>
   </si>
   <si>
-    <t>2016-09-05 10:18 AM</t>
+    <t>2016-09-05 20:21 PM</t>
   </si>
   <si>
     <t>用例总数</t>
@@ -102,13 +102,13 @@
     <t>内存占用峰值</t>
   </si>
   <si>
-    <t>3086M</t>
-  </si>
-  <si>
-    <t>内存平均使用情况</t>
-  </si>
-  <si>
-    <t>内存最大峰值</t>
+    <t>3014M</t>
+  </si>
+  <si>
+    <t>1%</t>
+  </si>
+  <si>
+    <t>76KB</t>
   </si>
   <si>
     <t>CPU</t>
@@ -123,10 +123,10 @@
     <t>8核</t>
   </si>
   <si>
-    <t>cpu平均使用情况</t>
-  </si>
-  <si>
-    <t>cpu最大峰值使用情况</t>
+    <t>67%</t>
+  </si>
+  <si>
+    <t>77%</t>
   </si>
   <si>
     <t>测试详情</t>
@@ -663,7 +663,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="3">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F6" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix get men error
</commit_message>
<xml_diff>
--- a/testRunner/report.xlsx
+++ b/testRunner/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>测试报告总概况</t>
   </si>
@@ -47,7 +47,7 @@
     <t>'2.2.8'</t>
   </si>
   <si>
-    <t>2016-09-05 20:21 PM</t>
+    <t>2016-09-06 20:06 PM</t>
   </si>
   <si>
     <t>用例总数</t>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>测试耗时</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
   <si>
     <t>脚本语言</t>
@@ -105,10 +108,10 @@
     <t>3014M</t>
   </si>
   <si>
-    <t>1%</t>
-  </si>
-  <si>
-    <t>76KB</t>
+    <t>23%</t>
+  </si>
+  <si>
+    <t>80742KB</t>
   </si>
   <si>
     <t>CPU</t>
@@ -123,10 +126,10 @@
     <t>8核</t>
   </si>
   <si>
-    <t>67%</t>
-  </si>
-  <si>
-    <t>77%</t>
+    <t>68%</t>
+  </si>
+  <si>
+    <t>80%</t>
   </si>
   <si>
     <t>测试详情</t>
@@ -172,9 +175,6 @@
   </si>
   <si>
     <t>test_home_shopcart</t>
-  </si>
-  <si>
-    <t>我的模块1</t>
   </si>
 </sst>
 </file>
@@ -611,10 +611,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -629,10 +629,10 @@
         <v>12</v>
       </c>
       <c r="E4" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1">
@@ -662,15 +662,15 @@
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3">
-        <v>57</v>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1"/>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -680,62 +680,62 @@
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1"/>
@@ -771,7 +771,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -781,22 +781,22 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1">
@@ -804,16 +804,16 @@
         <v>1001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -822,16 +822,16 @@
         <v>1004</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -840,73 +840,22 @@
         <v>1003</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="3">
-        <v>1001</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
-      <c r="A7" s="3">
-        <v>1004</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
-      <c r="A8" s="3">
-        <v>1003</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1"/>
+    <row r="7" spans="1:6" ht="30" customHeight="1"/>
+    <row r="8" spans="1:6" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
update dir shwo pic
</commit_message>
<xml_diff>
--- a/testRunner/report.xlsx
+++ b/testRunner/report.xlsx
@@ -47,7 +47,7 @@
     <t>'2.2.8'</t>
   </si>
   <si>
-    <t>2016-09-07 11:24 AM</t>
+    <t>2016-09-07 11:34 AM</t>
   </si>
   <si>
     <t>用例总数</t>
@@ -62,7 +62,7 @@
     <t>测试耗时</t>
   </si>
   <si>
-    <t>21</t>
+    <t>30</t>
   </si>
   <si>
     <t>脚本语言</t>
@@ -108,10 +108,10 @@
     <t>3014M</t>
   </si>
   <si>
-    <t>23%</t>
-  </si>
-  <si>
-    <t>78070KB</t>
+    <t>22%</t>
+  </si>
+  <si>
+    <t>77021KB</t>
   </si>
   <si>
     <t>CPU</t>
@@ -126,10 +126,10 @@
     <t>8核</t>
   </si>
   <si>
-    <t>36%</t>
-  </si>
-  <si>
-    <t>53%</t>
+    <t>63%</t>
+  </si>
+  <si>
+    <t>71%</t>
   </si>
   <si>
     <t>测试详情</t>

</xml_diff>